<commit_message>
Finished board. No errors remaining.
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>Component</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>https://www.digikey.ca/products/en?keywords=70543-0003</t>
+  </si>
+  <si>
+    <t>C1-8</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
   </si>
 </sst>
 </file>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,6 +938,14 @@
         <v>1.26</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>

</xml_diff>

<commit_message>
Added female connectors to BOM
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>Component</t>
   </si>
@@ -225,13 +225,43 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/te-connectivity-amp-connectors/2-644803-2/A30924-ND/698439</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>8-PDIP</t>
+  </si>
+  <si>
+    <t>3386P</t>
+  </si>
+  <si>
+    <t>8-SOIC (0.154", 3.90mm Width)</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>2 pin female connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/te-connectivity-amp-connectors/3-640441-2/A30978-ND/698221</t>
+  </si>
+  <si>
+    <t>4 pin female connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/te-connectivity-amp-connectors/3-640441-4/A30980-ND/698223</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,13 +289,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -277,17 +319,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -567,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="G16" sqref="G16:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +632,7 @@
     <col min="7" max="7" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -615,8 +663,11 @@
       <c r="J1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -635,7 +686,7 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H2">
@@ -648,11 +699,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
@@ -667,7 +718,7 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H3">
@@ -679,12 +730,15 @@
       <c r="J3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C4" t="s">
@@ -699,7 +753,7 @@
       <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H4">
@@ -711,12 +765,15 @@
       <c r="J4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C5" t="s">
@@ -731,7 +788,7 @@
       <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H5">
@@ -743,8 +800,11 @@
       <c r="J5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -754,7 +814,7 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H6">
@@ -766,8 +826,11 @@
       <c r="J6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -780,7 +843,7 @@
       <c r="E7" t="s">
         <v>39</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H7">
@@ -793,7 +856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -803,7 +866,7 @@
       <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="5" t="s">
         <v>66</v>
       </c>
       <c r="H8">
@@ -816,14 +879,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>52</v>
       </c>
       <c r="H9">
@@ -836,7 +899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -846,7 +909,7 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="H10">
@@ -859,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -869,7 +932,7 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H11">
@@ -882,7 +945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -892,7 +955,7 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="3" t="s">
         <v>55</v>
       </c>
       <c r="H12">
@@ -905,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -915,7 +978,7 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H13">
@@ -928,7 +991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -938,7 +1001,7 @@
       <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H14">
@@ -951,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -961,7 +1024,7 @@
       <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="3" t="s">
         <v>57</v>
       </c>
       <c r="H15">
@@ -972,13 +1035,54 @@
       </c>
       <c r="J15">
         <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16">
+        <v>0.24</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17">
+        <v>0.26</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>